<commit_message>
fixed table definition and default attribute NULL value handler
</commit_message>
<xml_diff>
--- a/documentation/SQL_tables.xlsx
+++ b/documentation/SQL_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\app-ts\c$\Users\adm_har3005\Documents\sources\git\AdTidy\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A6CCA3-3065-4DFE-9925-1455C7C16F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB538593-D9F2-4F0F-96BB-879B842640BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{3511F786-3003-4B1E-9A0A-339533652B0E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{3511F786-3003-4B1E-9A0A-339533652B0E}"/>
   </bookViews>
   <sheets>
     <sheet name="ADTidy_Inventory_Computers" sheetId="27" r:id="rId1"/>
@@ -2718,7 +2718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1EB3F9D-214D-478F-A637-26E1DD5C8C0E}">
   <dimension ref="A4:AR70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -16970,8 +16970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423B15E3-A192-417D-A481-DD02C91ADAB6}">
   <dimension ref="A4:AR70"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -18273,7 +18273,9 @@
         <v>94</v>
       </c>
       <c r="F16" s="29"/>
-      <c r="G16" s="37"/>
+      <c r="G16" s="37">
+        <v>1</v>
+      </c>
       <c r="H16" s="30"/>
       <c r="I16" s="38" t="s">
         <v>92</v>
@@ -18309,7 +18311,7 @@
       </c>
       <c r="T16" s="4" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v xml:space="preserve"> NOT NULL</v>
       </c>
       <c r="U16" s="4" t="str">
         <f t="shared" si="5"/>
@@ -18321,7 +18323,7 @@
       </c>
       <c r="Y16" t="str">
         <f t="shared" si="15"/>
-        <v>[ad_businessCategory] VARCHAR (MAX) ,</v>
+        <v>[ad_businessCategory] VARCHAR (MAX)  NOT NULL,</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" si="16"/>
@@ -18337,19 +18339,19 @@
       </c>
       <c r="AC16" s="68" t="str">
         <f t="shared" si="19"/>
-        <v/>
+        <v>"nullable": 1,</v>
       </c>
       <c r="AD16" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v xml:space="preserve"> NOT NULL</v>
       </c>
       <c r="AE16" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>{"name": "ad_businessCategory","type": "VARCHAR(MAX)"}</v>
+        <v>{"name": "ad_businessCategory","type": "VARCHAR(MAX)","nullable": 1}</v>
       </c>
       <c r="AF16" s="4" t="str">
         <f t="shared" si="21"/>
-        <v>{"name": "ad_businessCategory","type": "VARCHAR(MAX)"},</v>
+        <v>{"name": "ad_businessCategory","type": "VARCHAR(MAX)","nullable": 1},</v>
       </c>
       <c r="AG16" s="4" t="str">
         <f t="shared" si="8"/>
@@ -22989,7 +22991,7 @@
       </c>
       <c r="U53" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>,</v>
+        <v/>
       </c>
       <c r="V53" s="4" t="str">
         <f t="shared" si="6"/>
@@ -22997,7 +22999,7 @@
       </c>
       <c r="Y53" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">   ,</v>
+        <v xml:space="preserve">   </v>
       </c>
       <c r="Z53" t="str">
         <f t="shared" si="16"/>
@@ -23025,7 +23027,7 @@
       </c>
       <c r="AF53" s="4" t="str">
         <f t="shared" si="21"/>
-        <v>,</v>
+        <v/>
       </c>
       <c r="AG53" s="4" t="str">
         <f t="shared" si="8"/>
@@ -23070,14 +23072,12 @@
       </c>
     </row>
     <row r="54" spans="1:43" s="4" customFormat="1">
-      <c r="A54" s="24">
+      <c r="A54" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v/>
       </c>
       <c r="B54" s="25"/>
-      <c r="C54" s="26">
-        <v>9</v>
-      </c>
+      <c r="C54" s="26"/>
       <c r="D54" s="27"/>
       <c r="E54" s="28"/>
       <c r="F54" s="29"/>
@@ -23097,7 +23097,7 @@
       </c>
       <c r="P54" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>[9]</v>
+        <v/>
       </c>
       <c r="Q54" s="4" t="str">
         <f t="shared" si="26"/>
@@ -23125,11 +23125,11 @@
       </c>
       <c r="Y54" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">[9]   </v>
+        <v xml:space="preserve">   </v>
       </c>
       <c r="Z54" t="str">
         <f t="shared" si="16"/>
-        <v>{"name": "9",</v>
+        <v/>
       </c>
       <c r="AA54" t="str">
         <f t="shared" si="17"/>
@@ -23149,11 +23149,11 @@
       </c>
       <c r="AE54" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>{"name": "9"}</v>
+        <v/>
       </c>
       <c r="AF54" s="4" t="str">
         <f t="shared" si="21"/>
-        <v>{"name": "9"}</v>
+        <v/>
       </c>
       <c r="AG54" s="4" t="str">
         <f t="shared" si="8"/>
@@ -23833,7 +23833,7 @@
       </c>
       <c r="B60" s="72" t="str">
         <f>_xlfn.TEXTJOIN(,1,Y7:Y61)</f>
-        <v>CREATE TABLE [dbo].[ADTidy_Inventory_Organizational_Unit] ([record_source] VARCHAR (100) ,[record_lastupdate] DATETIME  ,[record_status] VARCHAR (50) ,[ad_whenCreated] DATETIME  ,[ad_whenChanged] DATETIME  ,[ad_distinguishedname] VARCHAR (MAX) ,[ad_objectguid] VARCHAR (50) ,[ad_name] VARCHAR (100) ,[ad_businessCategory] VARCHAR (MAX) ,[ad_managedBy] VARCHAR (MAX)  NOT NULL                                                                                                            ,[9]                  ) ON [PRIMARY]</v>
+        <v>CREATE TABLE [dbo].[ADTidy_Inventory_Organizational_Unit] ([record_source] VARCHAR (100) ,[record_lastupdate] DATETIME  ,[record_status] VARCHAR (50) ,[ad_whenCreated] DATETIME  ,[ad_whenChanged] DATETIME  ,[ad_distinguishedname] VARCHAR (MAX) ,[ad_objectguid] VARCHAR (50) ,[ad_name] VARCHAR (100) ,[ad_businessCategory] VARCHAR (MAX)  NOT NULL,[ad_managedBy] VARCHAR (MAX)  NOT NULL                                                                                                                              ) ON [PRIMARY]</v>
       </c>
       <c r="C60" s="72"/>
       <c r="D60" s="72"/>
@@ -23887,7 +23887,7 @@
       <c r="AC61" s="2"/>
       <c r="AF61" s="49" t="str">
         <f>_xlfn.TEXTJOIN(,1,AF6:AF60)</f>
-        <v>"Fields": [{"name": "record_source","type": "VARCHAR(100)"},{"name": "record_lastupdate","type": "DATETIME"},{"name": "record_status","type": "VARCHAR(50)"},{"name": "ad_whenCreated","type": "DATETIME"},{"name": "ad_whenChanged","type": "DATETIME"},{"name": "ad_distinguishedname","type": "VARCHAR(MAX)"},{"name": "ad_objectguid","type": "VARCHAR(50)"},{"name": "ad_name","type": "VARCHAR(100)"},{"name": "ad_businessCategory","type": "VARCHAR(MAX)"},{"name": "ad_managedBy","type": "VARCHAR(MAX)","nullable": 1},{"name": "9"}],</v>
+        <v>"Fields": [{"name": "record_source","type": "VARCHAR(100)"},{"name": "record_lastupdate","type": "DATETIME"},{"name": "record_status","type": "VARCHAR(50)"},{"name": "ad_whenCreated","type": "DATETIME"},{"name": "ad_whenChanged","type": "DATETIME"},{"name": "ad_distinguishedname","type": "VARCHAR(MAX)"},{"name": "ad_objectguid","type": "VARCHAR(50)"},{"name": "ad_name","type": "VARCHAR(100)"},{"name": "ad_businessCategory","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_managedBy","type": "VARCHAR(MAX)","nullable": 1}],</v>
       </c>
       <c r="AI61" s="45"/>
       <c r="AJ61" s="45"/>
@@ -23905,7 +23905,7 @@
       </c>
       <c r="B62" s="73" t="str">
         <f>"{"&amp;AF61&amp;AQ61&amp;"}"</f>
-        <v>{"Fields": [{"name": "record_source","type": "VARCHAR(100)"},{"name": "record_lastupdate","type": "DATETIME"},{"name": "record_status","type": "VARCHAR(50)"},{"name": "ad_whenCreated","type": "DATETIME"},{"name": "ad_whenChanged","type": "DATETIME"},{"name": "ad_distinguishedname","type": "VARCHAR(MAX)"},{"name": "ad_objectguid","type": "VARCHAR(50)"},{"name": "ad_name","type": "VARCHAR(100)"},{"name": "ad_businessCategory","type": "VARCHAR(MAX)"},{"name": "ad_managedBy","type": "VARCHAR(MAX)","nullable": 1},{"name": "9"}],"FieldsAssignement": [{"name": "record_source","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Calculation","Type": "record_source"}]}]},{"name": "record_lastupdate","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Calculation","Type": "current_datetime"}]}]},{"name": "record_status","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "status"}]}]},{"name": "ad_whenCreated","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "whenCreated"}]}]},{"name": "ad_whenChanged","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "whenChanged"}]}]},{"name": "ad_distinguishedname","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "distinguishedname"}]}]},{"name": "ad_objectguid","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "objectguid"}]}]},{"name": "ad_name","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "name"}]}]},{"name": "ad_businessCategory","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "businessCategory"}]}]},{"name": "ad_managedBy","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "ManagedBy"}]}]}]}</v>
+        <v>{"Fields": [{"name": "record_source","type": "VARCHAR(100)"},{"name": "record_lastupdate","type": "DATETIME"},{"name": "record_status","type": "VARCHAR(50)"},{"name": "ad_whenCreated","type": "DATETIME"},{"name": "ad_whenChanged","type": "DATETIME"},{"name": "ad_distinguishedname","type": "VARCHAR(MAX)"},{"name": "ad_objectguid","type": "VARCHAR(50)"},{"name": "ad_name","type": "VARCHAR(100)"},{"name": "ad_businessCategory","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_managedBy","type": "VARCHAR(MAX)","nullable": 1}],"FieldsAssignement": [{"name": "record_source","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Calculation","Type": "record_source"}]}]},{"name": "record_lastupdate","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Calculation","Type": "current_datetime"}]}]},{"name": "record_status","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "status"}]}]},{"name": "ad_whenCreated","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "whenCreated"}]}]},{"name": "ad_whenChanged","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "whenChanged"}]}]},{"name": "ad_distinguishedname","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "distinguishedname"}]}]},{"name": "ad_objectguid","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "objectguid"}]}]},{"name": "ad_name","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "name"}]}]},{"name": "ad_businessCategory","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "businessCategory"}]}]},{"name": "ad_managedBy","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "ManagedBy"}]}]}]}</v>
       </c>
       <c r="C62" s="73"/>
       <c r="D62" s="73"/>
@@ -23976,8 +23976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F984CED-F6E1-49B4-91B3-1C60D2ADC7AA}">
   <dimension ref="A4:AR70"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62:L63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -25561,7 +25561,9 @@
         <v>100</v>
       </c>
       <c r="F18" s="29"/>
-      <c r="G18" s="37"/>
+      <c r="G18" s="37">
+        <v>1</v>
+      </c>
       <c r="H18" s="30"/>
       <c r="I18" s="38" t="s">
         <v>88</v>
@@ -25597,7 +25599,7 @@
       </c>
       <c r="T18" s="4" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v xml:space="preserve"> NOT NULL</v>
       </c>
       <c r="U18" s="4" t="str">
         <f t="shared" si="5"/>
@@ -25609,7 +25611,7 @@
       </c>
       <c r="Y18" t="str">
         <f t="shared" si="15"/>
-        <v>[ad_userprincipalname] VARCHAR (100) ,</v>
+        <v>[ad_userprincipalname] VARCHAR (100)  NOT NULL,</v>
       </c>
       <c r="Z18" t="str">
         <f t="shared" si="16"/>
@@ -25625,19 +25627,19 @@
       </c>
       <c r="AC18" s="68" t="str">
         <f t="shared" si="19"/>
-        <v/>
+        <v>"nullable": 1,</v>
       </c>
       <c r="AD18" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v xml:space="preserve"> NOT NULL</v>
       </c>
       <c r="AE18" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>{"name": "ad_userprincipalname","type": "VARCHAR(100)"}</v>
+        <v>{"name": "ad_userprincipalname","type": "VARCHAR(100)","nullable": 1}</v>
       </c>
       <c r="AF18" s="4" t="str">
         <f t="shared" si="21"/>
-        <v>{"name": "ad_userprincipalname","type": "VARCHAR(100)"},</v>
+        <v>{"name": "ad_userprincipalname","type": "VARCHAR(100)","nullable": 1},</v>
       </c>
       <c r="AG18" s="4" t="str">
         <f t="shared" si="8"/>
@@ -26953,7 +26955,9 @@
         <v>97</v>
       </c>
       <c r="F28" s="29"/>
-      <c r="G28" s="37"/>
+      <c r="G28" s="37">
+        <v>1</v>
+      </c>
       <c r="H28" s="30"/>
       <c r="I28" s="38" t="s">
         <v>88</v>
@@ -26989,7 +26993,7 @@
       </c>
       <c r="T28" s="4" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v xml:space="preserve"> NOT NULL</v>
       </c>
       <c r="U28" s="4" t="str">
         <f t="shared" si="5"/>
@@ -27001,7 +27005,7 @@
       </c>
       <c r="Y28" t="str">
         <f t="shared" si="15"/>
-        <v>[ad_displayname] VARCHAR (50) ,</v>
+        <v>[ad_displayname] VARCHAR (50)  NOT NULL,</v>
       </c>
       <c r="Z28" t="str">
         <f t="shared" si="16"/>
@@ -27017,19 +27021,19 @@
       </c>
       <c r="AC28" s="68" t="str">
         <f t="shared" si="19"/>
-        <v/>
+        <v>"nullable": 1,</v>
       </c>
       <c r="AD28" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v xml:space="preserve"> NOT NULL</v>
       </c>
       <c r="AE28" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>{"name": "ad_displayname","type": "VARCHAR(50)"}</v>
+        <v>{"name": "ad_displayname","type": "VARCHAR(50)","nullable": 1}</v>
       </c>
       <c r="AF28" s="4" t="str">
         <f t="shared" si="21"/>
-        <v>{"name": "ad_displayname","type": "VARCHAR(50)"},</v>
+        <v>{"name": "ad_displayname","type": "VARCHAR(50)","nullable": 1},</v>
       </c>
       <c r="AG28" s="4" t="str">
         <f t="shared" si="8"/>
@@ -31405,7 +31409,7 @@
       </c>
       <c r="B60" s="72" t="str">
         <f>_xlfn.TEXTJOIN(,1,Y7:Y61)</f>
-        <v>CREATE TABLE [dbo].[ADTidy_Inventory_Users] ([record_source] VARCHAR (100) ,[record_lastupdate] DATETIME  ,[record_status] VARCHAR (50) ,[ad_whenCreated] DATETIME  ,[ad_whenChanged] DATETIME  ,[ad_distinguishedname] VARCHAR (MAX) ,[ad_lastlogontimestamp] DATETIME   NOT NULL,[ad_pwdLastSet] DATETIME   NOT NULL,[ad_extensionAttribute2] VARCHAR (50)  NOT NULL,[ad_samaccountname] VARCHAR (33) ,[ad_userprincipalname] VARCHAR (100) ,[ad_objectguid] VARCHAR (50) ,[ad_sid] VARCHAR (50) ,[ad_userAccountControl] VARCHAR (100) ,[ad_accountExpires] DATETIME   NOT NULL,[ad_extensionAttribute4] VARCHAR (20)  NOT NULL,[ad_extensionAttribute7] VARCHAR (MAX)  NOT NULL,[ad_givenName] VARCHAR (50)  NOT NULL,[ad_sn] VARCHAR (100)  NOT NULL,[ad_initials] VARCHAR (10)  NOT NULL,[ad_displayname] VARCHAR (50) ,[ad_division] VARCHAR (20)  NOT NULL,[ad_description] VARCHAR (MAX)  NOT NULL,[ad_info] VARCHAR (MAX)  NOT NULL,[ad_company] VARCHAR (100)  NOT NULL,[ad_department] VARCHAR (16)  NOT NULL,[ad_extensionAttribute5] VARCHAR (20)  NOT NULL,[ad_departmentnumber] VARCHAR (20)  NOT NULL,[ad_title] VARCHAR (50)  NOT NULL,[ad_employeeid] VARCHAR (30)  NOT NULL,[ad_employeetype] VARCHAR (30)  NOT NULL,[ad_extensionAttribute1] VARCHAR (70)  NOT NULL,[ad_manager] VARCHAR (MAX)  NOT NULL,[ad_thumbnailPhoto] VARCHAR (MAX)  NOT NULL,[ad_physicaldeliveryofficename] VARCHAR (100)  NOT NULL,[ad_streetaddress] VARCHAR (50)  NOT NULL,[ad_postalcode] VARCHAR (20)  NOT NULL,[ad_l] VARCHAR (50)  NOT NULL,[ad_c] VARCHAR (2)  NOT NULL,[ad_extensionAttribute3] VARCHAR (2)  NOT NULL,[ad_preferredLanguage] VARCHAR (30)  NOT NULL,[ad_telephonenumber] VARCHAR (50)  NOT NULL,[ad_mobile] VARCHAR (50)  NOT NULL,[ad_MsExchUserCulture] VARCHAR (30)  NOT NULL,[ad_mail] VARCHAR (100)  NOT NULL,[ad_homeMdb] VARCHAR (MAX)  NOT NULL,[ad_msExchMailboxGuid] VARCHAR (50)  NOT NULL,[ad_proxyaddresses] XML   NOT NULL,[ad_extensionAttribute6] VARCHAR (MAX)  NOT NULL,[az_MFA] XML   NOT NULL,[xml_extended_attributes] XML   NOT NULL   ) ON [PRIMARY]</v>
+        <v>CREATE TABLE [dbo].[ADTidy_Inventory_Users] ([record_source] VARCHAR (100) ,[record_lastupdate] DATETIME  ,[record_status] VARCHAR (50) ,[ad_whenCreated] DATETIME  ,[ad_whenChanged] DATETIME  ,[ad_distinguishedname] VARCHAR (MAX) ,[ad_lastlogontimestamp] DATETIME   NOT NULL,[ad_pwdLastSet] DATETIME   NOT NULL,[ad_extensionAttribute2] VARCHAR (50)  NOT NULL,[ad_samaccountname] VARCHAR (33) ,[ad_userprincipalname] VARCHAR (100)  NOT NULL,[ad_objectguid] VARCHAR (50) ,[ad_sid] VARCHAR (50) ,[ad_userAccountControl] VARCHAR (100) ,[ad_accountExpires] DATETIME   NOT NULL,[ad_extensionAttribute4] VARCHAR (20)  NOT NULL,[ad_extensionAttribute7] VARCHAR (MAX)  NOT NULL,[ad_givenName] VARCHAR (50)  NOT NULL,[ad_sn] VARCHAR (100)  NOT NULL,[ad_initials] VARCHAR (10)  NOT NULL,[ad_displayname] VARCHAR (50)  NOT NULL,[ad_division] VARCHAR (20)  NOT NULL,[ad_description] VARCHAR (MAX)  NOT NULL,[ad_info] VARCHAR (MAX)  NOT NULL,[ad_company] VARCHAR (100)  NOT NULL,[ad_department] VARCHAR (16)  NOT NULL,[ad_extensionAttribute5] VARCHAR (20)  NOT NULL,[ad_departmentnumber] VARCHAR (20)  NOT NULL,[ad_title] VARCHAR (50)  NOT NULL,[ad_employeeid] VARCHAR (30)  NOT NULL,[ad_employeetype] VARCHAR (30)  NOT NULL,[ad_extensionAttribute1] VARCHAR (70)  NOT NULL,[ad_manager] VARCHAR (MAX)  NOT NULL,[ad_thumbnailPhoto] VARCHAR (MAX)  NOT NULL,[ad_physicaldeliveryofficename] VARCHAR (100)  NOT NULL,[ad_streetaddress] VARCHAR (50)  NOT NULL,[ad_postalcode] VARCHAR (20)  NOT NULL,[ad_l] VARCHAR (50)  NOT NULL,[ad_c] VARCHAR (2)  NOT NULL,[ad_extensionAttribute3] VARCHAR (2)  NOT NULL,[ad_preferredLanguage] VARCHAR (30)  NOT NULL,[ad_telephonenumber] VARCHAR (50)  NOT NULL,[ad_mobile] VARCHAR (50)  NOT NULL,[ad_MsExchUserCulture] VARCHAR (30)  NOT NULL,[ad_mail] VARCHAR (100)  NOT NULL,[ad_homeMdb] VARCHAR (MAX)  NOT NULL,[ad_msExchMailboxGuid] VARCHAR (50)  NOT NULL,[ad_proxyaddresses] XML   NOT NULL,[ad_extensionAttribute6] VARCHAR (MAX)  NOT NULL,[az_MFA] XML   NOT NULL,[xml_extended_attributes] XML   NOT NULL   ) ON [PRIMARY]</v>
       </c>
       <c r="C60" s="72"/>
       <c r="D60" s="72"/>
@@ -31459,7 +31463,7 @@
       <c r="AC61" s="2"/>
       <c r="AF61" s="49" t="str">
         <f>_xlfn.TEXTJOIN(,1,AF6:AF60)</f>
-        <v>"Fields": [{"name": "record_source","type": "VARCHAR(100)"},{"name": "record_lastupdate","type": "DATETIME"},{"name": "record_status","type": "VARCHAR(50)"},{"name": "ad_whenCreated","type": "DATETIME"},{"name": "ad_whenChanged","type": "DATETIME"},{"name": "ad_distinguishedname","type": "VARCHAR(MAX)"},{"name": "ad_lastlogontimestamp","type": "DATETIME","nullable": 1},{"name": "ad_pwdLastSet","type": "DATETIME","nullable": 1},{"name": "ad_extensionAttribute2","type": "VARCHAR(50)","nullable": 1},{"name": "ad_samaccountname","type": "VARCHAR(33)"},{"name": "ad_userprincipalname","type": "VARCHAR(100)"},{"name": "ad_objectguid","type": "VARCHAR(50)"},{"name": "ad_sid","type": "VARCHAR(50)"},{"name": "ad_userAccountControl","type": "VARCHAR(100)"},{"name": "ad_accountExpires","type": "DATETIME","nullable": 1},{"name": "ad_extensionAttribute4","type": "VARCHAR(20)","nullable": 1},{"name": "ad_extensionAttribute7","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_givenName","type": "VARCHAR(50)","nullable": 1},{"name": "ad_sn","type": "VARCHAR(100)","nullable": 1},{"name": "ad_initials","type": "VARCHAR(10)","nullable": 1},{"name": "ad_displayname","type": "VARCHAR(50)"},{"name": "ad_division","type": "VARCHAR(20)","nullable": 1},{"name": "ad_description","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_info","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_company","type": "VARCHAR(100)","nullable": 1},{"name": "ad_department","type": "VARCHAR(16)","nullable": 1},{"name": "ad_extensionAttribute5","type": "VARCHAR(20)","nullable": 1},{"name": "ad_departmentnumber","type": "VARCHAR(20)","nullable": 1},{"name": "ad_title","type": "VARCHAR(50)","nullable": 1},{"name": "ad_employeeid","type": "VARCHAR(30)","nullable": 1},{"name": "ad_employeetype","type": "VARCHAR(30)","nullable": 1},{"name": "ad_extensionAttribute1","type": "VARCHAR(70)","nullable": 1},{"name": "ad_manager","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_thumbnailPhoto","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_physicaldeliveryofficename","type": "VARCHAR(100)","nullable": 1},{"name": "ad_streetaddress","type": "VARCHAR(50)","nullable": 1},{"name": "ad_postalcode","type": "VARCHAR(20)","nullable": 1},{"name": "ad_l","type": "VARCHAR(50)","nullable": 1},{"name": "ad_c","type": "VARCHAR(2)","nullable": 1},{"name": "ad_extensionAttribute3","type": "VARCHAR(2)","nullable": 1},{"name": "ad_preferredLanguage","type": "VARCHAR(30)","nullable": 1},{"name": "ad_telephonenumber","type": "VARCHAR(50)","nullable": 1},{"name": "ad_mobile","type": "VARCHAR(50)","nullable": 1},{"name": "ad_MsExchUserCulture","type": "VARCHAR(30)","nullable": 1},{"name": "ad_mail","type": "VARCHAR(100)","nullable": 1},{"name": "ad_homeMdb","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_msExchMailboxGuid","type": "VARCHAR(50)","nullable": 1},{"name": "ad_proxyaddresses","type": "XML","nullable": 1},{"name": "ad_extensionAttribute6","type": "VARCHAR(MAX)","nullable": 1},{"name": "az_MFA","type": "XML","nullable": 1},{"name": "xml_extended_attributes","type": "XML","nullable": 1}],</v>
+        <v>"Fields": [{"name": "record_source","type": "VARCHAR(100)"},{"name": "record_lastupdate","type": "DATETIME"},{"name": "record_status","type": "VARCHAR(50)"},{"name": "ad_whenCreated","type": "DATETIME"},{"name": "ad_whenChanged","type": "DATETIME"},{"name": "ad_distinguishedname","type": "VARCHAR(MAX)"},{"name": "ad_lastlogontimestamp","type": "DATETIME","nullable": 1},{"name": "ad_pwdLastSet","type": "DATETIME","nullable": 1},{"name": "ad_extensionAttribute2","type": "VARCHAR(50)","nullable": 1},{"name": "ad_samaccountname","type": "VARCHAR(33)"},{"name": "ad_userprincipalname","type": "VARCHAR(100)","nullable": 1},{"name": "ad_objectguid","type": "VARCHAR(50)"},{"name": "ad_sid","type": "VARCHAR(50)"},{"name": "ad_userAccountControl","type": "VARCHAR(100)"},{"name": "ad_accountExpires","type": "DATETIME","nullable": 1},{"name": "ad_extensionAttribute4","type": "VARCHAR(20)","nullable": 1},{"name": "ad_extensionAttribute7","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_givenName","type": "VARCHAR(50)","nullable": 1},{"name": "ad_sn","type": "VARCHAR(100)","nullable": 1},{"name": "ad_initials","type": "VARCHAR(10)","nullable": 1},{"name": "ad_displayname","type": "VARCHAR(50)","nullable": 1},{"name": "ad_division","type": "VARCHAR(20)","nullable": 1},{"name": "ad_description","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_info","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_company","type": "VARCHAR(100)","nullable": 1},{"name": "ad_department","type": "VARCHAR(16)","nullable": 1},{"name": "ad_extensionAttribute5","type": "VARCHAR(20)","nullable": 1},{"name": "ad_departmentnumber","type": "VARCHAR(20)","nullable": 1},{"name": "ad_title","type": "VARCHAR(50)","nullable": 1},{"name": "ad_employeeid","type": "VARCHAR(30)","nullable": 1},{"name": "ad_employeetype","type": "VARCHAR(30)","nullable": 1},{"name": "ad_extensionAttribute1","type": "VARCHAR(70)","nullable": 1},{"name": "ad_manager","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_thumbnailPhoto","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_physicaldeliveryofficename","type": "VARCHAR(100)","nullable": 1},{"name": "ad_streetaddress","type": "VARCHAR(50)","nullable": 1},{"name": "ad_postalcode","type": "VARCHAR(20)","nullable": 1},{"name": "ad_l","type": "VARCHAR(50)","nullable": 1},{"name": "ad_c","type": "VARCHAR(2)","nullable": 1},{"name": "ad_extensionAttribute3","type": "VARCHAR(2)","nullable": 1},{"name": "ad_preferredLanguage","type": "VARCHAR(30)","nullable": 1},{"name": "ad_telephonenumber","type": "VARCHAR(50)","nullable": 1},{"name": "ad_mobile","type": "VARCHAR(50)","nullable": 1},{"name": "ad_MsExchUserCulture","type": "VARCHAR(30)","nullable": 1},{"name": "ad_mail","type": "VARCHAR(100)","nullable": 1},{"name": "ad_homeMdb","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_msExchMailboxGuid","type": "VARCHAR(50)","nullable": 1},{"name": "ad_proxyaddresses","type": "XML","nullable": 1},{"name": "ad_extensionAttribute6","type": "VARCHAR(MAX)","nullable": 1},{"name": "az_MFA","type": "XML","nullable": 1},{"name": "xml_extended_attributes","type": "XML","nullable": 1}],</v>
       </c>
       <c r="AI61" s="45"/>
       <c r="AJ61" s="45"/>
@@ -31477,7 +31481,7 @@
       </c>
       <c r="B62" s="73" t="str">
         <f>"{"&amp;AF61&amp;AQ61&amp;"}"</f>
-        <v>{"Fields": [{"name": "record_source","type": "VARCHAR(100)"},{"name": "record_lastupdate","type": "DATETIME"},{"name": "record_status","type": "VARCHAR(50)"},{"name": "ad_whenCreated","type": "DATETIME"},{"name": "ad_whenChanged","type": "DATETIME"},{"name": "ad_distinguishedname","type": "VARCHAR(MAX)"},{"name": "ad_lastlogontimestamp","type": "DATETIME","nullable": 1},{"name": "ad_pwdLastSet","type": "DATETIME","nullable": 1},{"name": "ad_extensionAttribute2","type": "VARCHAR(50)","nullable": 1},{"name": "ad_samaccountname","type": "VARCHAR(33)"},{"name": "ad_userprincipalname","type": "VARCHAR(100)"},{"name": "ad_objectguid","type": "VARCHAR(50)"},{"name": "ad_sid","type": "VARCHAR(50)"},{"name": "ad_userAccountControl","type": "VARCHAR(100)"},{"name": "ad_accountExpires","type": "DATETIME","nullable": 1},{"name": "ad_extensionAttribute4","type": "VARCHAR(20)","nullable": 1},{"name": "ad_extensionAttribute7","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_givenName","type": "VARCHAR(50)","nullable": 1},{"name": "ad_sn","type": "VARCHAR(100)","nullable": 1},{"name": "ad_initials","type": "VARCHAR(10)","nullable": 1},{"name": "ad_displayname","type": "VARCHAR(50)"},{"name": "ad_division","type": "VARCHAR(20)","nullable": 1},{"name": "ad_description","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_info","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_company","type": "VARCHAR(100)","nullable": 1},{"name": "ad_department","type": "VARCHAR(16)","nullable": 1},{"name": "ad_extensionAttribute5","type": "VARCHAR(20)","nullable": 1},{"name": "ad_departmentnumber","type": "VARCHAR(20)","nullable": 1},{"name": "ad_title","type": "VARCHAR(50)","nullable": 1},{"name": "ad_employeeid","type": "VARCHAR(30)","nullable": 1},{"name": "ad_employeetype","type": "VARCHAR(30)","nullable": 1},{"name": "ad_extensionAttribute1","type": "VARCHAR(70)","nullable": 1},{"name": "ad_manager","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_thumbnailPhoto","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_physicaldeliveryofficename","type": "VARCHAR(100)","nullable": 1},{"name": "ad_streetaddress","type": "VARCHAR(50)","nullable": 1},{"name": "ad_postalcode","type": "VARCHAR(20)","nullable": 1},{"name": "ad_l","type": "VARCHAR(50)","nullable": 1},{"name": "ad_c","type": "VARCHAR(2)","nullable": 1},{"name": "ad_extensionAttribute3","type": "VARCHAR(2)","nullable": 1},{"name": "ad_preferredLanguage","type": "VARCHAR(30)","nullable": 1},{"name": "ad_telephonenumber","type": "VARCHAR(50)","nullable": 1},{"name": "ad_mobile","type": "VARCHAR(50)","nullable": 1},{"name": "ad_MsExchUserCulture","type": "VARCHAR(30)","nullable": 1},{"name": "ad_mail","type": "VARCHAR(100)","nullable": 1},{"name": "ad_homeMdb","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_msExchMailboxGuid","type": "VARCHAR(50)","nullable": 1},{"name": "ad_proxyaddresses","type": "XML","nullable": 1},{"name": "ad_extensionAttribute6","type": "VARCHAR(MAX)","nullable": 1},{"name": "az_MFA","type": "XML","nullable": 1},{"name": "xml_extended_attributes","type": "XML","nullable": 1}],"FieldsAssignement": [{"name": "record_source","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Calculation","Type": "record_source"}]}]},{"name": "record_lastupdate","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Calculation","Type": "current_datetime"}]}]},{"name": "record_status","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "status"}]}]},{"name": "ad_whenCreated","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "whenCreated"}]}]},{"name": "ad_whenChanged","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "whenChanged"}]}]},{"name": "ad_distinguishedname","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "distinguishedname"}]}]},{"name": "ad_lastlogontimestamp","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "lastlogontimestamp"}]}]},{"name": "ad_pwdLastSet","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Calculation","Type": "pwdLastSet"}]}]},{"name": "ad_extensionAttribute2","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "extensionattribute2"}]}]},{"name": "ad_samaccountname","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "samaccountname"}]}]},{"name": "ad_userprincipalname","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "userprincipalname"}]}]},{"name": "ad_objectguid","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "objectguid"}]}]},{"name": "ad_sid","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "SID"}]}]},{"name": "ad_userAccountControl","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Calculation","Type": "useraccountcontrol"}]}]},{"name": "ad_accountExpires","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Calculation","Type": "accountexpires"}]}]},{"name": "ad_extensionAttribute4","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "extensionAttribute4"}]}]},{"name": "ad_extensionAttribute7","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "extensionAttribute7"}]}]},{"name": "ad_givenName","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "givenName"}]}]},{"name": "ad_sn","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "sn"}]}]},{"name": "ad_initials","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "initials"}]}]},{"name": "ad_displayname","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "displayname"}]}]},{"name": "ad_division","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "division"}]}]},{"name": "ad_description","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "description"}]}]},{"name": "ad_info","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "info"}]}]},{"name": "ad_company","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "company"}]}]},{"name": "ad_department","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "department"}]}]},{"name": "ad_extensionAttribute5","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "extensionattribute5"}]}]},{"name": "ad_departmentnumber","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "departmentnumber"}]}]},{"name": "ad_title","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "title"}]}]},{"name": "ad_employeeid","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "employeeid"}]}]},{"name": "ad_employeetype","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "employeetype"}]}]},{"name": "ad_extensionAttribute1","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "extensionattribute1"}]}]},{"name": "ad_manager","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "manager"}]}]},{"name": "ad_thumbnailPhoto","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Calculation","Type": "thumbnailPhoto"}]}]},{"name": "ad_physicaldeliveryofficename","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "physicaldeliveryofficename"}]}]},{"name": "ad_streetaddress","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "streeatddress"}]}]},{"name": "ad_postalcode","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "postalcode"}]}]},{"name": "ad_l","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "l"}]}]},{"name": "ad_c","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "c"}]}]},{"name": "ad_extensionAttribute3","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "extensionAttribute3"}]}]},{"name": "ad_preferredLanguage","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "preferredLanguage"}]}]},{"name": "ad_telephonenumber","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "telephonenumber"}]}]},{"name": "ad_mobile","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "mobile"}]}]},{"name": "ad_MsExchUserCulture","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "MsExchUserCulture"}]}]},{"name": "ad_mail","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "mail"}]}]},{"name": "ad_homeMdb","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "homeMdb"}]}]},{"name": "ad_msExchMailboxGuid","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "msExchMailboxGuid"}]}]},{"name": "ad_proxyaddresses","Recipe":[{"ORDER":"1", "Content": [ {"Source": "","Type": ""}]}]},{"name": "ad_extensionAttribute6","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "extensionattribute6"}]}]},{"name": "az_MFA","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "mfa"}]}]},{"name": "xml_extended_attributes","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "xml_extended_attributes"}]}]}]}</v>
+        <v>{"Fields": [{"name": "record_source","type": "VARCHAR(100)"},{"name": "record_lastupdate","type": "DATETIME"},{"name": "record_status","type": "VARCHAR(50)"},{"name": "ad_whenCreated","type": "DATETIME"},{"name": "ad_whenChanged","type": "DATETIME"},{"name": "ad_distinguishedname","type": "VARCHAR(MAX)"},{"name": "ad_lastlogontimestamp","type": "DATETIME","nullable": 1},{"name": "ad_pwdLastSet","type": "DATETIME","nullable": 1},{"name": "ad_extensionAttribute2","type": "VARCHAR(50)","nullable": 1},{"name": "ad_samaccountname","type": "VARCHAR(33)"},{"name": "ad_userprincipalname","type": "VARCHAR(100)","nullable": 1},{"name": "ad_objectguid","type": "VARCHAR(50)"},{"name": "ad_sid","type": "VARCHAR(50)"},{"name": "ad_userAccountControl","type": "VARCHAR(100)"},{"name": "ad_accountExpires","type": "DATETIME","nullable": 1},{"name": "ad_extensionAttribute4","type": "VARCHAR(20)","nullable": 1},{"name": "ad_extensionAttribute7","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_givenName","type": "VARCHAR(50)","nullable": 1},{"name": "ad_sn","type": "VARCHAR(100)","nullable": 1},{"name": "ad_initials","type": "VARCHAR(10)","nullable": 1},{"name": "ad_displayname","type": "VARCHAR(50)","nullable": 1},{"name": "ad_division","type": "VARCHAR(20)","nullable": 1},{"name": "ad_description","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_info","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_company","type": "VARCHAR(100)","nullable": 1},{"name": "ad_department","type": "VARCHAR(16)","nullable": 1},{"name": "ad_extensionAttribute5","type": "VARCHAR(20)","nullable": 1},{"name": "ad_departmentnumber","type": "VARCHAR(20)","nullable": 1},{"name": "ad_title","type": "VARCHAR(50)","nullable": 1},{"name": "ad_employeeid","type": "VARCHAR(30)","nullable": 1},{"name": "ad_employeetype","type": "VARCHAR(30)","nullable": 1},{"name": "ad_extensionAttribute1","type": "VARCHAR(70)","nullable": 1},{"name": "ad_manager","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_thumbnailPhoto","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_physicaldeliveryofficename","type": "VARCHAR(100)","nullable": 1},{"name": "ad_streetaddress","type": "VARCHAR(50)","nullable": 1},{"name": "ad_postalcode","type": "VARCHAR(20)","nullable": 1},{"name": "ad_l","type": "VARCHAR(50)","nullable": 1},{"name": "ad_c","type": "VARCHAR(2)","nullable": 1},{"name": "ad_extensionAttribute3","type": "VARCHAR(2)","nullable": 1},{"name": "ad_preferredLanguage","type": "VARCHAR(30)","nullable": 1},{"name": "ad_telephonenumber","type": "VARCHAR(50)","nullable": 1},{"name": "ad_mobile","type": "VARCHAR(50)","nullable": 1},{"name": "ad_MsExchUserCulture","type": "VARCHAR(30)","nullable": 1},{"name": "ad_mail","type": "VARCHAR(100)","nullable": 1},{"name": "ad_homeMdb","type": "VARCHAR(MAX)","nullable": 1},{"name": "ad_msExchMailboxGuid","type": "VARCHAR(50)","nullable": 1},{"name": "ad_proxyaddresses","type": "XML","nullable": 1},{"name": "ad_extensionAttribute6","type": "VARCHAR(MAX)","nullable": 1},{"name": "az_MFA","type": "XML","nullable": 1},{"name": "xml_extended_attributes","type": "XML","nullable": 1}],"FieldsAssignement": [{"name": "record_source","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Calculation","Type": "record_source"}]}]},{"name": "record_lastupdate","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Calculation","Type": "current_datetime"}]}]},{"name": "record_status","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "status"}]}]},{"name": "ad_whenCreated","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "whenCreated"}]}]},{"name": "ad_whenChanged","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "whenChanged"}]}]},{"name": "ad_distinguishedname","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "distinguishedname"}]}]},{"name": "ad_lastlogontimestamp","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "lastlogontimestamp"}]}]},{"name": "ad_pwdLastSet","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Calculation","Type": "pwdLastSet"}]}]},{"name": "ad_extensionAttribute2","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "extensionattribute2"}]}]},{"name": "ad_samaccountname","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "samaccountname"}]}]},{"name": "ad_userprincipalname","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "userprincipalname"}]}]},{"name": "ad_objectguid","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "objectguid"}]}]},{"name": "ad_sid","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "SID"}]}]},{"name": "ad_userAccountControl","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Calculation","Type": "useraccountcontrol"}]}]},{"name": "ad_accountExpires","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Calculation","Type": "accountexpires"}]}]},{"name": "ad_extensionAttribute4","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "extensionAttribute4"}]}]},{"name": "ad_extensionAttribute7","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "extensionAttribute7"}]}]},{"name": "ad_givenName","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "givenName"}]}]},{"name": "ad_sn","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "sn"}]}]},{"name": "ad_initials","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "initials"}]}]},{"name": "ad_displayname","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "displayname"}]}]},{"name": "ad_division","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "division"}]}]},{"name": "ad_description","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "description"}]}]},{"name": "ad_info","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "info"}]}]},{"name": "ad_company","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "company"}]}]},{"name": "ad_department","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "department"}]}]},{"name": "ad_extensionAttribute5","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "extensionattribute5"}]}]},{"name": "ad_departmentnumber","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "departmentnumber"}]}]},{"name": "ad_title","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "title"}]}]},{"name": "ad_employeeid","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "employeeid"}]}]},{"name": "ad_employeetype","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "employeetype"}]}]},{"name": "ad_extensionAttribute1","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "extensionattribute1"}]}]},{"name": "ad_manager","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "manager"}]}]},{"name": "ad_thumbnailPhoto","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Calculation","Type": "thumbnailPhoto"}]}]},{"name": "ad_physicaldeliveryofficename","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "physicaldeliveryofficename"}]}]},{"name": "ad_streetaddress","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "streeatddress"}]}]},{"name": "ad_postalcode","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "postalcode"}]}]},{"name": "ad_l","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "l"}]}]},{"name": "ad_c","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "c"}]}]},{"name": "ad_extensionAttribute3","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "extensionAttribute3"}]}]},{"name": "ad_preferredLanguage","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "preferredLanguage"}]}]},{"name": "ad_telephonenumber","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "telephonenumber"}]}]},{"name": "ad_mobile","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "mobile"}]}]},{"name": "ad_MsExchUserCulture","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "MsExchUserCulture"}]}]},{"name": "ad_mail","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "mail"}]}]},{"name": "ad_homeMdb","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "homeMdb"}]}]},{"name": "ad_msExchMailboxGuid","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "msExchMailboxGuid"}]}]},{"name": "ad_proxyaddresses","Recipe":[{"ORDER":"1", "Content": [ {"Source": "","Type": ""}]}]},{"name": "ad_extensionAttribute6","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "extensionattribute6"}]}]},{"name": "az_MFA","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "mfa"}]}]},{"name": "xml_extended_attributes","Recipe":[{"ORDER":"1", "Content": [ {"Source": "Field","Type": "xml_extended_attributes"}]}]}]}</v>
       </c>
       <c r="C62" s="73"/>
       <c r="D62" s="73"/>
@@ -39070,6 +39074,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b72ab2fb-6c5f-42e9-80bb-f43e7ab8cfcd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9e3746d1-c0f6-44f4-a580-8db545e24bdc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101007A0671A7CFC0904FA8B28CF39620F29F" ma:contentTypeVersion="14" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="72ea80b52863a369c81d13747cb14fb8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b72ab2fb-6c5f-42e9-80bb-f43e7ab8cfcd" xmlns:ns3="9e3746d1-c0f6-44f4-a580-8db545e24bdc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3a303289134a2943eaf32359c5cb0726" ns2:_="" ns3:_="">
     <xsd:import namespace="b72ab2fb-6c5f-42e9-80bb-f43e7ab8cfcd"/>
@@ -39298,27 +39322,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b72ab2fb-6c5f-42e9-80bb-f43e7ab8cfcd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9e3746d1-c0f6-44f4-a580-8db545e24bdc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D37CAF3A-F7E8-454A-8004-B0CA273E018C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9e3746d1-c0f6-44f4-a580-8db545e24bdc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="b72ab2fb-6c5f-42e9-80bb-f43e7ab8cfcd"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{031359E4-B9CE-44D2-96B1-828F36D93122}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5657DF4-5FDD-4765-AAC2-42F03D1E7EDA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -39335,29 +39364,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D37CAF3A-F7E8-454A-8004-B0CA273E018C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9e3746d1-c0f6-44f4-a580-8db545e24bdc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="b72ab2fb-6c5f-42e9-80bb-f43e7ab8cfcd"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{031359E4-B9CE-44D2-96B1-828F36D93122}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>